<commit_message>
Add Properties File Logic
</commit_message>
<xml_diff>
--- a/bin/Test.xlsx
+++ b/bin/Test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>ElementName</t>
   </si>
@@ -76,12 +76,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>u_0_7</t>
-  </si>
-  <si>
-    <t>u_0_9</t>
-  </si>
-  <si>
     <t>rgba(0, 0, 0, 1)</t>
   </si>
   <si>
@@ -113,6 +107,18 @@
   </si>
   <si>
     <t>TC_1</t>
+  </si>
+  <si>
+    <t>xLocation</t>
+  </si>
+  <si>
+    <t>yLocation</t>
+  </si>
+  <si>
+    <t>u_0_1</t>
+  </si>
+  <si>
+    <t>u_0_3</t>
   </si>
 </sst>
 </file>
@@ -981,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,7 +1007,7 @@
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1035,8 +1041,14 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1050,28 +1062,34 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>872</v>
+      </c>
+      <c r="M2">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1085,28 +1103,34 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="L3">
+        <v>1036</v>
+      </c>
+      <c r="M3">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1117,31 +1141,37 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>849</v>
+      </c>
+      <c r="M4">
+        <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1152,28 +1182,34 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>1054</v>
+      </c>
+      <c r="M5">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>